<commit_message>
changes to dataLog, added logs for data set 2
</commit_message>
<xml_diff>
--- a/Etude09_PulsesCounting/dataLog.xlsx
+++ b/Etude09_PulsesCounting/dataLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\Desktop\University\COSC326\PairEtudes\Etude09_PulsesCounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E122FB5-52B9-42EA-BE71-D4D2A7EC44F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA54C22-66C1-4A79-BB04-AAADC3DA9AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{DEF670DB-88E8-4D47-9FDD-42560624FB67}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="pulseData2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1868,7 +1867,7 @@
   <dimension ref="A1:N201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C2" sqref="C2:C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,9 +1876,6 @@
       <c r="A1" s="1">
         <v>1.49278483780315E-5</v>
       </c>
-      <c r="C1">
-        <v>788</v>
-      </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
@@ -1901,7 +1897,7 @@
         <v>1.9741734931179899E-4</v>
       </c>
       <c r="C2">
-        <v>761</v>
+        <v>788</v>
       </c>
       <c r="E2">
         <v>15.1520041113271</v>
@@ -1924,7 +1920,7 @@
         <v>1.16078692139372E-3</v>
       </c>
       <c r="C3">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E3">
         <v>4.5587463815742604</v>
@@ -1947,7 +1943,7 @@
         <v>3.8001846212089899E-3</v>
       </c>
       <c r="C4">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="E4">
         <v>-15.214460724821899</v>
@@ -1970,7 +1966,7 @@
         <v>6.4151997677601097E-3</v>
       </c>
       <c r="C5">
-        <v>726</v>
+        <v>754</v>
       </c>
       <c r="E5">
         <v>-29.7684468875335</v>
@@ -1993,7 +1989,7 @@
         <v>-8.9996028800470797E-4</v>
       </c>
       <c r="C6">
-        <v>751</v>
+        <v>726</v>
       </c>
       <c r="E6">
         <v>-25.3191411785863</v>
@@ -2016,7 +2012,7 @@
         <v>-3.3983856797701599E-2</v>
       </c>
       <c r="C7">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E7">
         <v>-0.76038450925937895</v>
@@ -2039,7 +2035,7 @@
         <v>-8.6865654185678196E-2</v>
       </c>
       <c r="C8">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="E8">
         <v>28.012597141543999</v>
@@ -2062,7 +2058,7 @@
         <v>-8.9062802240866698E-2</v>
       </c>
       <c r="C9">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="E9">
         <v>39.505250921320503</v>
@@ -2085,7 +2081,7 @@
         <v>7.9813931589673301E-2</v>
       </c>
       <c r="C10">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="E10">
         <v>25.2046469004164</v>
@@ -2108,7 +2104,7 @@
         <v>0.44039337839450399</v>
       </c>
       <c r="C11">
-        <v>795</v>
+        <v>759</v>
       </c>
       <c r="E11">
         <v>-3.16538190418833</v>
@@ -2131,7 +2127,7 @@
         <v>0.70469195930644701</v>
       </c>
       <c r="C12">
-        <v>774</v>
+        <v>795</v>
       </c>
       <c r="E12">
         <v>-24.783945460671699</v>
@@ -2154,7 +2150,7 @@
         <v>0.30762696218999602</v>
       </c>
       <c r="C13">
-        <v>757</v>
+        <v>774</v>
       </c>
       <c r="E13">
         <v>-27.204478119698301</v>
@@ -2177,7 +2173,7 @@
         <v>-1.06108908802321</v>
       </c>
       <c r="C14">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="E14">
         <v>-13.5525945359432</v>
@@ -2200,7 +2196,7 @@
         <v>-2.6903882837787498</v>
       </c>
       <c r="C15">
-        <v>757</v>
+        <v>763</v>
       </c>
       <c r="E15">
         <v>4.0102247885942104</v>
@@ -2223,7 +2219,7 @@
         <v>-2.7492226282088099</v>
       </c>
       <c r="C16">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E16">
         <v>14.938347252486601</v>
@@ -2246,7 +2242,7 @@
         <v>0.37293073659897602</v>
       </c>
       <c r="C17">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E17">
         <v>15.633098890102699</v>
@@ -2269,7 +2265,7 @@
         <v>5.8490110078209598</v>
       </c>
       <c r="C18">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E18">
         <v>8.4926963928111707</v>
@@ -2292,7 +2288,7 @@
         <v>9.4658082410281903</v>
       </c>
       <c r="C19">
-        <v>792</v>
+        <v>759</v>
       </c>
       <c r="E19">
         <v>-1.2758225855124801</v>
@@ -2315,7 +2311,7 @@
         <v>6.0006569554136604</v>
       </c>
       <c r="C20">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="E20">
         <v>-8.44258207397543</v>
@@ -2338,7 +2334,7 @@
         <v>-5.6995572286069098</v>
       </c>
       <c r="C21">
-        <v>760</v>
+        <v>783</v>
       </c>
       <c r="E21">
         <v>-9.9145717802690108</v>
@@ -2361,7 +2357,7 @@
         <v>-19.045909434787799</v>
       </c>
       <c r="C22">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="E22">
         <v>-5.9850418046413498</v>
@@ -2384,7 +2380,7 @@
         <v>-22.1851204473815</v>
       </c>
       <c r="C23">
-        <v>757</v>
+        <v>772</v>
       </c>
       <c r="E23">
         <v>0.221171107867211</v>
@@ -2407,7 +2403,7 @@
         <v>-7.0792996559644301</v>
       </c>
       <c r="C24">
-        <v>805</v>
+        <v>757</v>
       </c>
       <c r="E24">
         <v>4.9660318792479599</v>
@@ -2430,7 +2426,7 @@
         <v>21.0404240875068</v>
       </c>
       <c r="C25">
-        <v>748</v>
+        <v>805</v>
       </c>
       <c r="E25">
         <v>6.1408329477524397</v>
@@ -2453,7 +2449,7 @@
         <v>43.013123378751303</v>
       </c>
       <c r="C26">
-        <v>760</v>
+        <v>748</v>
       </c>
       <c r="E26">
         <v>4.0088021711573196</v>
@@ -2476,7 +2472,7 @@
         <v>37.835491794868197</v>
       </c>
       <c r="C27">
-        <v>787</v>
+        <v>760</v>
       </c>
       <c r="E27">
         <v>0.40272273458246999</v>
@@ -2499,7 +2495,7 @@
         <v>0.58357509964952203</v>
       </c>
       <c r="C28">
-        <v>800</v>
+        <v>787</v>
       </c>
       <c r="E28">
         <v>-2.62061719394592</v>
@@ -2522,7 +2518,7 @@
         <v>-48.355568043383798</v>
       </c>
       <c r="C29">
-        <v>772</v>
+        <v>800</v>
       </c>
       <c r="E29">
         <v>-3.7930448736131801</v>
@@ -2545,7 +2541,7 @@
         <v>-73.415233719535607</v>
       </c>
       <c r="C30">
-        <v>830</v>
+        <v>772</v>
       </c>
       <c r="E30">
         <v>-3.0071529142995401</v>
@@ -2568,7 +2564,7 @@
         <v>-49.405049641683803</v>
       </c>
       <c r="C31">
-        <v>725</v>
+        <v>830</v>
       </c>
       <c r="E31">
         <v>-1.0764085785259301</v>
@@ -2591,7 +2587,7 @@
         <v>15.860156736798499</v>
       </c>
       <c r="C32">
-        <v>763</v>
+        <v>725</v>
       </c>
       <c r="E32">
         <v>0.89765973763736695</v>
@@ -2637,7 +2633,7 @@
         <v>99.413229771779896</v>
       </c>
       <c r="C34">
-        <v>742</v>
+        <v>763</v>
       </c>
       <c r="E34">
         <v>2.4064041732913402</v>
@@ -2660,7 +2656,7 @@
         <v>50.824434095742298</v>
       </c>
       <c r="C35">
-        <v>721</v>
+        <v>742</v>
       </c>
       <c r="E35">
         <v>1.82856941293765</v>
@@ -2683,7 +2679,7 @@
         <v>-37.098492344961599</v>
       </c>
       <c r="C36">
-        <v>810</v>
+        <v>721</v>
       </c>
       <c r="E36">
         <v>0.65937559530033296</v>
@@ -2706,7 +2702,7 @@
         <v>-106.660776902481</v>
       </c>
       <c r="C37">
-        <v>780</v>
+        <v>810</v>
       </c>
       <c r="E37">
         <v>-0.75231473968294604</v>
@@ -2729,7 +2725,7 @@
         <v>-109.635854005482</v>
       </c>
       <c r="C38">
-        <v>759</v>
+        <v>780</v>
       </c>
       <c r="E38">
         <v>-1.90841136237036</v>
@@ -2775,7 +2771,7 @@
         <v>51.626034843529901</v>
       </c>
       <c r="C40">
-        <v>752</v>
+        <v>759</v>
       </c>
       <c r="E40">
         <v>-1.5355175096726701</v>
@@ -2798,7 +2794,7 @@
         <v>110.706795565584</v>
       </c>
       <c r="C41">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E41">
         <v>2.4968744994381301E-2</v>
@@ -2821,7 +2817,7 @@
         <v>99.397818743710502</v>
       </c>
       <c r="C42">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="E42">
         <v>1.6428186530412101</v>
@@ -2844,7 +2840,7 @@
         <v>30.188346081717899</v>
       </c>
       <c r="C43">
-        <v>752</v>
+        <v>759</v>
       </c>
       <c r="E43">
         <v>2.4040989051785999</v>
@@ -2867,7 +2863,7 @@
         <v>-48.588632802396603</v>
       </c>
       <c r="C44">
-        <v>804</v>
+        <v>752</v>
       </c>
       <c r="E44">
         <v>1.8010412988014299</v>
@@ -2890,7 +2886,7 @@
         <v>-88.666936760611307</v>
       </c>
       <c r="C45">
-        <v>794</v>
+        <v>804</v>
       </c>
       <c r="E45">
         <v>0.100236984261327</v>
@@ -2913,7 +2909,7 @@
         <v>-73.433915278811099</v>
       </c>
       <c r="C46">
-        <v>759</v>
+        <v>794</v>
       </c>
       <c r="E46">
         <v>-1.74055758894668</v>
@@ -2936,7 +2932,7 @@
         <v>-23.2467984701135</v>
       </c>
       <c r="C47">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E47">
         <v>-2.6119012402940398</v>
@@ -2959,7 +2955,7 @@
         <v>25.433238292922301</v>
       </c>
       <c r="C48">
-        <v>752</v>
+        <v>760</v>
       </c>
       <c r="E48">
         <v>-1.9387839963484801</v>
@@ -2982,7 +2978,7 @@
         <v>47.573441500407696</v>
       </c>
       <c r="C49">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="E49">
         <v>-7.0115040615714094E-2</v>
@@ -3005,7 +3001,7 @@
         <v>42.389878777581401</v>
       </c>
       <c r="C50">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E50">
         <v>1.9025315100595801</v>
@@ -3051,7 +3047,7 @@
         <v>9.6216257717236804</v>
       </c>
       <c r="C52">
-        <v>784</v>
+        <v>752</v>
       </c>
       <c r="E52">
         <v>2.07721904102105</v>
@@ -3074,7 +3070,7 @@
         <v>-2.3864902148796499</v>
       </c>
       <c r="C53">
-        <v>801</v>
+        <v>784</v>
       </c>
       <c r="E53">
         <v>0.145420873114912</v>
@@ -3097,7 +3093,7 @@
         <v>-16.2080247137459</v>
       </c>
       <c r="C54">
-        <v>760</v>
+        <v>801</v>
       </c>
       <c r="E54">
         <v>-1.8770304673132301</v>
@@ -3120,7 +3116,7 @@
         <v>-32.585236011713697</v>
       </c>
       <c r="C55">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E55">
         <v>-2.83072351571011</v>
@@ -3143,7 +3139,7 @@
         <v>-42.062941165399103</v>
       </c>
       <c r="C56">
-        <v>754</v>
+        <v>762</v>
       </c>
       <c r="E56">
         <v>-2.1769750103410801</v>
@@ -3166,7 +3162,7 @@
         <v>-32.148541626199297</v>
       </c>
       <c r="C57">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="E57">
         <v>-0.28860609450345498</v>
@@ -3189,7 +3185,7 @@
         <v>-0.68645750641016401</v>
       </c>
       <c r="C58">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="E58">
         <v>1.7674387026919101</v>
@@ -3235,7 +3231,7 @@
         <v>59.246869200972199</v>
       </c>
       <c r="C60">
-        <v>800</v>
+        <v>753</v>
       </c>
       <c r="E60">
         <v>2.2593078300457998</v>
@@ -3258,7 +3254,7 @@
         <v>48.343535613112003</v>
       </c>
       <c r="C61">
-        <v>795</v>
+        <v>800</v>
       </c>
       <c r="E61">
         <v>0.37676368990745202</v>
@@ -3281,7 +3277,7 @@
         <v>9.6393440249072402</v>
       </c>
       <c r="C62">
-        <v>762</v>
+        <v>795</v>
       </c>
       <c r="E62">
         <v>-1.75155480525123</v>
@@ -3304,7 +3300,7 @@
         <v>-33.975393993371497</v>
       </c>
       <c r="C63">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="E63">
         <v>-2.8758541729029101</v>
@@ -3327,7 +3323,7 @@
         <v>-56.832320877093601</v>
       </c>
       <c r="C64">
-        <v>754</v>
+        <v>761</v>
       </c>
       <c r="E64">
         <v>-2.3041532387079902</v>
@@ -3350,7 +3346,7 @@
         <v>-47.394497471909801</v>
       </c>
       <c r="C65">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="E65">
         <v>-0.34039494831632999</v>
@@ -3373,7 +3369,7 @@
         <v>-14.415296285590401</v>
       </c>
       <c r="C66">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="E66">
         <v>1.85820468785394</v>
@@ -3396,7 +3392,7 @@
         <v>20.9492346814691</v>
       </c>
       <c r="C67">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="E67">
         <v>2.9530576698866899</v>
@@ -3419,7 +3415,7 @@
         <v>39.856798539532697</v>
       </c>
       <c r="C68">
-        <v>817</v>
+        <v>762</v>
       </c>
       <c r="E68">
         <v>2.2418602546050299</v>
@@ -3442,7 +3438,7 @@
         <v>36.3194681037956</v>
       </c>
       <c r="C69">
-        <v>785</v>
+        <v>817</v>
       </c>
       <c r="E69">
         <v>0.120860205035054</v>
@@ -3465,7 +3461,7 @@
         <v>17.469737823656398</v>
       </c>
       <c r="C70">
-        <v>761</v>
+        <v>785</v>
       </c>
       <c r="E70">
         <v>-2.1187338898324799</v>
@@ -3488,7 +3484,7 @@
         <v>-4.1002233589193802</v>
       </c>
       <c r="C71">
-        <v>746</v>
+        <v>761</v>
       </c>
       <c r="E71">
         <v>-3.0688788762974002</v>
@@ -3511,7 +3507,7 @@
         <v>-18.694500843193101</v>
       </c>
       <c r="C72">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E72">
         <v>-2.0950876097268099</v>
@@ -3534,7 +3530,7 @@
         <v>-23.0054318719184</v>
       </c>
       <c r="C73">
-        <v>761</v>
+        <v>748</v>
       </c>
       <c r="E73">
         <v>0.22589799842578601</v>
@@ -3557,7 +3553,7 @@
         <v>-18.5479691145594</v>
       </c>
       <c r="C74">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="E74">
         <v>2.4344485139226499</v>
@@ -3580,7 +3576,7 @@
         <v>-8.6273738134440894</v>
       </c>
       <c r="C75">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="E75">
         <v>3.1140634542852998</v>
@@ -3603,7 +3599,7 @@
         <v>3.1062928493311399</v>
       </c>
       <c r="C76">
-        <v>814</v>
+        <v>760</v>
       </c>
       <c r="E76">
         <v>1.8264145892489001</v>
@@ -3626,7 +3622,7 @@
         <v>12.6134703495169</v>
       </c>
       <c r="C77">
-        <v>748</v>
+        <v>814</v>
       </c>
       <c r="E77">
         <v>-0.58581211813780298</v>
@@ -3649,7 +3645,7 @@
         <v>16.004980434509498</v>
       </c>
       <c r="C78">
-        <v>758</v>
+        <v>748</v>
       </c>
       <c r="E78">
         <v>-2.5608050491379402</v>
@@ -3672,7 +3668,7 @@
         <v>11.6250642983779</v>
       </c>
       <c r="C79">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E79">
         <v>-2.8646578450690998</v>
@@ -3695,7 +3691,7 @@
         <v>2.0237432316663102</v>
       </c>
       <c r="C80">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="E80">
         <v>-1.3894625711879101</v>
@@ -3718,7 +3714,7 @@
         <v>-6.7729167834048098</v>
       </c>
       <c r="C81">
-        <v>769</v>
+        <v>750</v>
       </c>
       <c r="E81">
         <v>0.84085198955951201</v>
@@ -3741,7 +3737,7 @@
         <v>-9.1857563983659301</v>
       </c>
       <c r="C82">
-        <v>747</v>
+        <v>769</v>
       </c>
       <c r="E82">
         <v>2.41234121145943</v>
@@ -3764,7 +3760,7 @@
         <v>-4.4379100258539097</v>
       </c>
       <c r="C83">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="E83">
         <v>2.4447990524729599</v>
@@ -3787,7 +3783,7 @@
         <v>2.5186762037363701</v>
       </c>
       <c r="C84">
-        <v>795</v>
+        <v>751</v>
       </c>
       <c r="E84">
         <v>1.0654632785021401</v>
@@ -3810,7 +3806,7 @@
         <v>4.8641780589604897</v>
       </c>
       <c r="C85">
-        <v>786</v>
+        <v>795</v>
       </c>
       <c r="E85">
         <v>-0.806034852371036</v>
@@ -3833,7 +3829,7 @@
         <v>-0.237668974208288</v>
       </c>
       <c r="C86">
-        <v>759</v>
+        <v>786</v>
       </c>
       <c r="E86">
         <v>-2.10049961686628</v>
@@ -3856,7 +3852,7 @@
         <v>-8.70135035506412</v>
       </c>
       <c r="C87">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E87">
         <v>-2.19349250133157</v>
@@ -3879,7 +3875,7 @@
         <v>-12.351188916900099</v>
       </c>
       <c r="C88">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="E88">
         <v>-1.13994194495291</v>
@@ -3902,7 +3898,7 @@
         <v>-5.6625277002584804</v>
       </c>
       <c r="C89">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="E89">
         <v>0.45524088267048701</v>
@@ -3925,7 +3921,7 @@
         <v>8.92907747416311</v>
       </c>
       <c r="C90">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="E90">
         <v>1.7688912123166001</v>
@@ -3948,7 +3944,7 @@
         <v>21.720666400678901</v>
       </c>
       <c r="C91">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="E91">
         <v>2.1436968908392502</v>
@@ -3971,7 +3967,7 @@
         <v>22.432409473990599</v>
       </c>
       <c r="C92">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="E92">
         <v>1.40412886740954</v>
@@ -3994,7 +3990,7 @@
         <v>8.0996260428662694</v>
       </c>
       <c r="C93">
-        <v>784</v>
+        <v>758</v>
       </c>
       <c r="E93">
         <v>-3.9710282565067402E-2</v>
@@ -4017,7 +4013,7 @@
         <v>-13.8302807143377</v>
       </c>
       <c r="C94">
-        <v>765</v>
+        <v>784</v>
       </c>
       <c r="E94">
         <v>-1.40306205087252</v>
@@ -4040,7 +4036,7 @@
         <v>-29.808717218731001</v>
       </c>
       <c r="C95">
-        <v>760</v>
+        <v>765</v>
       </c>
       <c r="E95">
         <v>-1.9685205959423699</v>
@@ -4086,7 +4082,7 @@
         <v>-11.1517139137614</v>
       </c>
       <c r="C97">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="E97">
         <v>-0.27575032158044799</v>
@@ -4109,7 +4105,7 @@
         <v>13.789264468275301</v>
       </c>
       <c r="C98">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E98">
         <v>0.99589747161359399</v>
@@ -4132,7 +4128,7 @@
         <v>31.059733779473301</v>
       </c>
       <c r="C99">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="E99">
         <v>1.6879735111196299</v>
@@ -4155,7 +4151,7 @@
         <v>30.769620781556501</v>
       </c>
       <c r="C100">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="E100">
         <v>1.4870523270076299</v>
@@ -4178,7 +4174,7 @@
         <v>13.667907644121</v>
       </c>
       <c r="C101">
-        <v>794</v>
+        <v>761</v>
       </c>
       <c r="E101">
         <v>0.52564446569648404</v>
@@ -4201,7 +4197,7 @@
         <v>-9.8288786762225602</v>
       </c>
       <c r="C102">
-        <v>774</v>
+        <v>794</v>
       </c>
       <c r="E102">
         <v>-0.69679133705776697</v>
@@ -4224,7 +4220,7 @@
         <v>-26.388476715159399</v>
       </c>
       <c r="C103">
-        <v>761</v>
+        <v>774</v>
       </c>
       <c r="E103">
         <v>-1.5489697468568999</v>
@@ -4247,7 +4243,7 @@
         <v>-27.688281853060801</v>
       </c>
       <c r="C104">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E104">
         <v>-1.574009831106</v>
@@ -4270,7 +4266,7 @@
         <v>-14.6289863838514</v>
       </c>
       <c r="C105">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="E105">
         <v>-0.73492855168467297</v>
@@ -4293,7 +4289,7 @@
         <v>4.2414225906240404</v>
       </c>
       <c r="C106">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E106">
         <v>0.53696886679857403</v>
@@ -4316,7 +4312,7 @@
         <v>18.4296560758936</v>
       </c>
       <c r="C107">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="E107">
         <v>1.54713508240564</v>
@@ -4339,7 +4335,7 @@
         <v>21.450675431394998</v>
       </c>
       <c r="C108">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="E108">
         <v>1.71130181865331</v>
@@ -4362,7 +4358,7 @@
         <v>13.618070155958399</v>
       </c>
       <c r="C109">
-        <v>805</v>
+        <v>764</v>
       </c>
       <c r="E109">
         <v>0.89615468539114296</v>
@@ -4385,7 +4381,7 @@
         <v>0.67053872656327196</v>
       </c>
       <c r="C110">
-        <v>786</v>
+        <v>805</v>
       </c>
       <c r="E110">
         <v>-0.47707955930688101</v>
@@ -4408,7 +4404,7 @@
         <v>-10.2091243808198</v>
       </c>
       <c r="C111">
-        <v>761</v>
+        <v>786</v>
       </c>
       <c r="E111">
         <v>-1.64296730217913</v>
@@ -4431,7 +4427,7 @@
         <v>-14.289213440406799</v>
       </c>
       <c r="C112">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E112">
         <v>-1.91209634035583</v>
@@ -4454,7 +4450,7 @@
         <v>-11.063423376926</v>
       </c>
       <c r="C113">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c r="E113">
         <v>-1.07372453927927</v>
@@ -4477,7 +4473,7 @@
         <v>-3.5178118744876499</v>
       </c>
       <c r="C114">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E114">
         <v>0.448023629011219</v>
@@ -4500,7 +4496,7 @@
         <v>4.0729030084928901</v>
       </c>
       <c r="C115">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E115">
         <v>1.7945818358624901</v>
@@ -4523,7 +4519,7 @@
         <v>8.3455088830866497</v>
       </c>
       <c r="C116">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E116">
         <v>2.1485035473471701</v>
@@ -4546,7 +4542,7 @@
         <v>8.0590081336270707</v>
       </c>
       <c r="C117">
-        <v>807</v>
+        <v>761</v>
       </c>
       <c r="E117">
         <v>1.2273732275379701</v>
@@ -4569,7 +4565,7 @@
         <v>4.1361459615145497</v>
       </c>
       <c r="C118">
-        <v>799</v>
+        <v>807</v>
       </c>
       <c r="E118">
         <v>-0.50360491134949903</v>
@@ -4592,7 +4588,7 @@
         <v>-1.1031409922436599</v>
       </c>
       <c r="C119">
-        <v>763</v>
+        <v>799</v>
       </c>
       <c r="E119">
         <v>-2.0534376517394901</v>
@@ -4615,7 +4611,7 @@
         <v>-5.0468608865371003</v>
       </c>
       <c r="C120">
-        <v>725</v>
+        <v>763</v>
       </c>
       <c r="E120">
         <v>-2.4594189132905599</v>
@@ -4638,7 +4634,7 @@
         <v>-5.8765005359512097</v>
       </c>
       <c r="C121">
-        <v>753</v>
+        <v>725</v>
       </c>
       <c r="E121">
         <v>-1.370674611511</v>
@@ -4661,7 +4657,7 @@
         <v>-3.3430684637364698</v>
       </c>
       <c r="C122">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E122">
         <v>0.67760255482998299</v>
@@ -4684,7 +4680,7 @@
         <v>1.0656722695258201</v>
       </c>
       <c r="C123">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="E123">
         <v>2.4995450082587198</v>
@@ -4707,7 +4703,7 @@
         <v>4.7730093547439498</v>
       </c>
       <c r="C124">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E124">
         <v>2.9342643029720601</v>
@@ -4730,7 +4726,7 @@
         <v>5.44256213452097</v>
       </c>
       <c r="C125">
-        <v>821</v>
+        <v>752</v>
       </c>
       <c r="E125">
         <v>1.5938206819307501</v>
@@ -4753,7 +4749,7 @@
         <v>2.38653062364763</v>
       </c>
       <c r="C126">
-        <v>784</v>
+        <v>821</v>
       </c>
       <c r="E126">
         <v>-0.81347066567033499</v>
@@ -4776,7 +4772,7 @@
         <v>-2.7958532595999199</v>
       </c>
       <c r="C127">
-        <v>759</v>
+        <v>784</v>
       </c>
       <c r="E127">
         <v>-2.8640138305875</v>
@@ -4799,7 +4795,7 @@
         <v>-6.9154269980822702</v>
       </c>
       <c r="C128">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E128">
         <v>-3.30162409399769</v>
@@ -4822,7 +4818,7 @@
         <v>-7.0224435187557503</v>
       </c>
       <c r="C129">
-        <v>752</v>
+        <v>763</v>
       </c>
       <c r="E129">
         <v>-1.8370129321353199</v>
@@ -4845,7 +4841,7 @@
         <v>-2.3610061131870999</v>
       </c>
       <c r="C130">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="E130">
         <v>0.67543886357832095</v>
@@ -4868,7 +4864,7 @@
         <v>4.8164335823043798</v>
       </c>
       <c r="C131">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="E131">
         <v>2.7833161565762898</v>
@@ -4891,7 +4887,7 @@
         <v>10.272210288550999</v>
       </c>
       <c r="C132">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E132">
         <v>3.3208546628620099</v>
@@ -4914,7 +4910,7 @@
         <v>10.2250164790611</v>
       </c>
       <c r="C133">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="E133">
         <v>2.0640685646477599</v>
@@ -4937,7 +4933,7 @@
         <v>3.8167800599798398</v>
       </c>
       <c r="C134">
-        <v>807</v>
+        <v>758</v>
       </c>
       <c r="E134">
         <v>-0.21505996503663899</v>
@@ -4960,7 +4956,7 @@
         <v>-5.9594469519923896</v>
       </c>
       <c r="C135">
-        <v>774</v>
+        <v>807</v>
       </c>
       <c r="E135">
         <v>-2.2606511332622099</v>
@@ -4983,7 +4979,7 @@
         <v>-13.6241545614328</v>
       </c>
       <c r="C136">
-        <v>757</v>
+        <v>774</v>
       </c>
       <c r="E136">
         <v>-3.0447148766849002</v>
@@ -5006,7 +5002,7 @@
         <v>-14.268915985824099</v>
       </c>
       <c r="C137">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="E137">
         <v>-2.2599536038959198</v>
@@ -5029,7 +5025,7 @@
         <v>-6.6107893597202096</v>
       </c>
       <c r="C138">
-        <v>749</v>
+        <v>760</v>
       </c>
       <c r="E138">
         <v>-0.38673836516581001</v>
@@ -5052,7 +5048,7 @@
         <v>5.8112763610297797</v>
       </c>
       <c r="C139">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="E139">
         <v>1.6059393317339701</v>
@@ -5075,7 +5071,7 @@
         <v>16.215077758853699</v>
       </c>
       <c r="C140">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E140">
         <v>2.7328698373403602</v>
@@ -5098,7 +5094,7 @@
         <v>18.277383283976501</v>
       </c>
       <c r="C141">
-        <v>760</v>
+        <v>753</v>
       </c>
       <c r="E141">
         <v>2.44554693329053</v>
@@ -5121,7 +5117,7 @@
         <v>9.9672654867469905</v>
       </c>
       <c r="C142">
-        <v>798</v>
+        <v>760</v>
       </c>
       <c r="E142">
         <v>0.89844233747882396</v>
@@ -5144,7 +5140,7 @@
         <v>-4.7876592070280601</v>
       </c>
       <c r="C143">
-        <v>785</v>
+        <v>798</v>
       </c>
       <c r="E143">
         <v>-1.1056434373891999</v>
@@ -5167,7 +5163,7 @@
         <v>-17.8619630258057</v>
       </c>
       <c r="C144">
-        <v>758</v>
+        <v>785</v>
       </c>
       <c r="E144">
         <v>-2.5100799768707698</v>
@@ -5190,7 +5186,7 @@
         <v>-21.4350714146067</v>
       </c>
       <c r="C145">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="E145">
         <v>-2.5629698214349799</v>
@@ -5213,7 +5209,7 @@
         <v>-12.7618881618783</v>
       </c>
       <c r="C146">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="E146">
         <v>-1.2329875740410701</v>
@@ -5259,7 +5255,7 @@
         <v>18.655648649406299</v>
       </c>
       <c r="C148">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="E148">
         <v>2.34159643096522</v>
@@ -5282,7 +5278,7 @@
         <v>23.067076101613701</v>
       </c>
       <c r="C149">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="E149">
         <v>2.64098837876735</v>
@@ -5305,7 +5301,7 @@
         <v>14.0533582446523</v>
       </c>
       <c r="C150">
-        <v>806</v>
+        <v>756</v>
       </c>
       <c r="E150">
         <v>1.48784246253688</v>
@@ -5328,7 +5324,7 @@
         <v>-3.2447439989328299</v>
       </c>
       <c r="C151">
-        <v>800</v>
+        <v>806</v>
       </c>
       <c r="E151">
         <v>-0.50092972744870501</v>
@@ -5351,7 +5347,7 @@
         <v>-18.575275012939802</v>
       </c>
       <c r="C152">
-        <v>764</v>
+        <v>800</v>
       </c>
       <c r="E152">
         <v>-2.2436429944096998</v>
@@ -5374,7 +5370,7 @@
         <v>-22.830595442039499</v>
       </c>
       <c r="C153">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E153">
         <v>-2.77270312928075</v>
@@ -5397,7 +5393,7 @@
         <v>-13.6668463112537</v>
       </c>
       <c r="C154">
-        <v>757</v>
+        <v>765</v>
       </c>
       <c r="E154">
         <v>-1.7625362618965801</v>
@@ -5420,7 +5416,7 @@
         <v>3.1355483594011702</v>
       </c>
       <c r="C155">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="E155">
         <v>0.271408557721873</v>
@@ -5443,7 +5439,7 @@
         <v>17.416809272501698</v>
       </c>
       <c r="C156">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E156">
         <v>2.21972027558036</v>
@@ -5489,7 +5485,7 @@
         <v>12.4061458336994</v>
       </c>
       <c r="C158">
-        <v>816</v>
+        <v>758</v>
       </c>
       <c r="E158">
         <v>2.0289800177936002</v>
@@ -5512,7 +5508,7 @@
         <v>-2.58105672119751</v>
       </c>
       <c r="C159">
-        <v>809</v>
+        <v>816</v>
       </c>
       <c r="E159">
         <v>-0.13506666111662199</v>
@@ -5535,7 +5531,7 @@
         <v>-15.075045608578799</v>
       </c>
       <c r="C160">
-        <v>769</v>
+        <v>809</v>
       </c>
       <c r="E160">
         <v>-2.3220024468524398</v>
@@ -5558,7 +5554,7 @@
         <v>-18.411918407548001</v>
       </c>
       <c r="C161">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="E161">
         <v>-3.2453071833685598</v>
@@ -5581,7 +5577,7 @@
         <v>-11.6364647804147</v>
       </c>
       <c r="C162">
-        <v>740</v>
+        <v>763</v>
       </c>
       <c r="E162">
         <v>-2.2895549711211198</v>
@@ -5604,7 +5600,7 @@
         <v>0.72809823378518601</v>
       </c>
       <c r="C163">
-        <v>747</v>
+        <v>740</v>
       </c>
       <c r="E163">
         <v>7.2362885459030496E-2</v>
@@ -5627,7 +5623,7 @@
         <v>11.8346613549575</v>
       </c>
       <c r="C164">
-        <v>797</v>
+        <v>747</v>
       </c>
       <c r="E164">
         <v>2.4843912610719201</v>
@@ -5650,7 +5646,7 @@
         <v>16.288629824764701</v>
       </c>
       <c r="C165">
-        <v>732</v>
+        <v>797</v>
       </c>
       <c r="E165">
         <v>3.4817293361051198</v>
@@ -5673,7 +5669,7 @@
         <v>12.4673422623321</v>
       </c>
       <c r="C166">
-        <v>793</v>
+        <v>732</v>
       </c>
       <c r="E166">
         <v>2.4062204545445498</v>
@@ -5696,7 +5692,7 @@
         <v>2.6709381827165402</v>
       </c>
       <c r="C167">
-        <v>806</v>
+        <v>793</v>
       </c>
       <c r="E167">
         <v>-0.134954851361445</v>
@@ -5719,7 +5715,7 @@
         <v>-8.3357027760254301</v>
       </c>
       <c r="C168">
-        <v>759</v>
+        <v>806</v>
       </c>
       <c r="E168">
         <v>-2.6218918981548098</v>
@@ -5742,7 +5738,7 @@
         <v>-15.419083120524199</v>
       </c>
       <c r="C169">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E169">
         <v>-3.5770870435430999</v>
@@ -5765,7 +5761,7 @@
         <v>-15.104105472532799</v>
       </c>
       <c r="C170">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="E170">
         <v>-2.4662534910253902</v>
@@ -5788,7 +5784,7 @@
         <v>-7.0928282327635701</v>
       </c>
       <c r="C171">
-        <v>709</v>
+        <v>749</v>
       </c>
       <c r="E171">
         <v>4.5501930966555602E-2</v>
@@ -5811,7 +5807,7 @@
         <v>5.2265821577663401</v>
       </c>
       <c r="C172">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="E172">
         <v>2.5625647146350499</v>
@@ -5834,7 +5830,7 @@
         <v>15.840970299812501</v>
       </c>
       <c r="C173">
-        <v>741</v>
+        <v>723</v>
       </c>
       <c r="E173">
         <v>3.7560742682344399</v>
@@ -5857,7 +5853,7 @@
         <v>18.810431139375599</v>
       </c>
       <c r="C174">
-        <v>769</v>
+        <v>741</v>
       </c>
       <c r="E174">
         <v>3.0124965562437902</v>
@@ -5880,7 +5876,7 @@
         <v>11.603055331438799</v>
       </c>
       <c r="C175">
-        <v>806</v>
+        <v>769</v>
       </c>
       <c r="E175">
         <v>0.68653270798311705</v>
@@ -5903,7 +5899,7 @@
         <v>-2.8323979583597301</v>
       </c>
       <c r="C176">
-        <v>770</v>
+        <v>806</v>
       </c>
       <c r="E176">
         <v>-2.0665503436180499</v>
@@ -5926,7 +5922,7 @@
         <v>-16.9357718170879</v>
       </c>
       <c r="C177">
-        <v>757</v>
+        <v>770</v>
       </c>
       <c r="E177">
         <v>-3.81602760252887</v>
@@ -5972,7 +5968,7 @@
         <v>-15.3482929573163</v>
       </c>
       <c r="C179">
-        <v>785</v>
+        <v>757</v>
       </c>
       <c r="E179">
         <v>-1.4449413709609999</v>
@@ -5995,7 +5991,7 @@
         <v>1.15274225405985</v>
       </c>
       <c r="C180">
-        <v>738</v>
+        <v>785</v>
       </c>
       <c r="E180">
         <v>1.4229377979226201</v>
@@ -6018,7 +6014,7 @@
         <v>17.929136176167201</v>
       </c>
       <c r="C181">
-        <v>765</v>
+        <v>738</v>
       </c>
       <c r="E181">
         <v>3.3873739211528</v>
@@ -6041,7 +6037,7 @@
         <v>25.0428881248971</v>
       </c>
       <c r="C182">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="E182">
         <v>3.3639987537587701</v>
@@ -6064,7 +6060,7 @@
         <v>17.803717152747801</v>
       </c>
       <c r="C183">
-        <v>804</v>
+        <v>762</v>
       </c>
       <c r="E183">
         <v>1.48318478528022</v>
@@ -6087,7 +6083,7 @@
         <v>-5.4331895173497402E-2</v>
       </c>
       <c r="C184">
-        <v>765</v>
+        <v>804</v>
       </c>
       <c r="E184">
         <v>-1.0469811664128501</v>
@@ -6110,7 +6106,7 @@
         <v>-18.277059399495101</v>
       </c>
       <c r="C185">
-        <v>760</v>
+        <v>765</v>
       </c>
       <c r="E185">
         <v>-2.7471765945044999</v>
@@ -6133,7 +6129,7 @@
         <v>-26.1182777926707</v>
       </c>
       <c r="C186">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E186">
         <v>-2.7487065667802999</v>
@@ -6156,7 +6152,7 @@
         <v>-18.846626941041499</v>
       </c>
       <c r="C187">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E187">
         <v>-1.2038913985572099</v>
@@ -6179,7 +6175,7 @@
         <v>-0.674403645654997</v>
       </c>
       <c r="C188">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="E188">
         <v>0.91409884229692695</v>
@@ -6202,7 +6198,7 @@
         <v>17.747933575454201</v>
       </c>
       <c r="C189">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="E189">
         <v>2.3968649946046101</v>
@@ -6225,7 +6221,7 @@
         <v>25.721880452299398</v>
       </c>
       <c r="C190">
-        <v>795</v>
+        <v>754</v>
       </c>
       <c r="E190">
         <v>2.4364333871768502</v>
@@ -6248,7 +6244,7 @@
         <v>18.826340984134799</v>
       </c>
       <c r="C191">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="E191">
         <v>1.03390528492964</v>
@@ -6271,7 +6267,7 @@
         <v>1.3598701652268499</v>
       </c>
       <c r="C192">
-        <v>771</v>
+        <v>801</v>
       </c>
       <c r="E192">
         <v>-0.99574336562236099</v>
@@ -6294,7 +6290,7 @@
         <v>-16.424138348729901</v>
       </c>
       <c r="C193">
-        <v>761</v>
+        <v>771</v>
       </c>
       <c r="E193">
         <v>-2.4542306391691899</v>
@@ -6317,7 +6313,7 @@
         <v>-24.4309392088478</v>
       </c>
       <c r="C194">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="E194">
         <v>-2.4406871813217199</v>
@@ -6340,7 +6336,7 @@
         <v>-18.461316965219002</v>
       </c>
       <c r="C195">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="E195">
         <v>-0.90936302058581897</v>
@@ -6363,7 +6359,7 @@
         <v>-2.31595988178332</v>
       </c>
       <c r="C196">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="E196">
         <v>1.2568254036850799</v>
@@ -6386,7 +6382,7 @@
         <v>14.681881333708199</v>
       </c>
       <c r="C197">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="E197">
         <v>2.7556722470436599</v>
@@ -6409,7 +6405,7 @@
         <v>23.073029072938901</v>
       </c>
       <c r="C198">
-        <v>806</v>
+        <v>754</v>
       </c>
       <c r="E198">
         <v>2.67711842471804</v>
@@ -6432,7 +6428,7 @@
         <v>18.4426938963298</v>
       </c>
       <c r="C199">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="E199">
         <v>1.1079226908028901</v>
@@ -6455,7 +6451,7 @@
         <v>3.63723239714062</v>
       </c>
       <c r="C200">
-        <v>771</v>
+        <v>812</v>
       </c>
       <c r="E200">
         <v>-0.89738635640332198</v>
@@ -6474,6 +6470,9 @@
       </c>
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C201">
+        <v>771</v>
+      </c>
       <c r="E201">
         <v>-1.9942459268997199</v>
       </c>

</xml_diff>